<commit_message>
mejoras dos hojas excel
</commit_message>
<xml_diff>
--- a/files/aaa_test.xlsx
+++ b/files/aaa_test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Python\Ejercicios\facturacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{897184DF-74D6-4834-8080-B9EEFDBF7DBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75F6D2D4-A27E-40D6-A940-26C4338A6416}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{59A3F954-9994-4991-B83A-6053DB489A6B}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="4">
   <si>
     <t>TX</t>
   </si>
@@ -37,6 +37,9 @@
   </si>
   <si>
     <t>LS1</t>
+  </si>
+  <si>
+    <t>LOTE TEST</t>
   </si>
 </sst>
 </file>
@@ -464,7 +467,7 @@
   <dimension ref="A1:F952"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="A10:B11"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -571,8 +574,12 @@
       <c r="F9" s="7"/>
     </row>
     <row r="10" spans="1:6" ht="15">
-      <c r="A10" s="5"/>
-      <c r="B10" s="3"/>
+      <c r="A10" s="5">
+        <v>99999999</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>3</v>
+      </c>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="F10" s="7"/>

</xml_diff>